<commit_message>
Add link to Figure A3.1
</commit_message>
<xml_diff>
--- a/reference-files/figures-template-provisional.xlsx
+++ b/reference-files/figures-template-provisional.xlsx
@@ -49,14 +49,14 @@
     <definedName name="_xlnm.Print_Area" localSheetId="10">'Figure 5 Background Data'!$B$2:$J$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'Figure A3.1'!$B$1:$L$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">OFFSET('Figure A3.1 Background Data'!$B$1:$H$1, 0, 0, calculation!$B$7+14, 9)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Notes!$A$1:$P$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Notes!$A$1:$P$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="162">
   <si>
     <t>External causes of death excluded from analysis</t>
   </si>
@@ -566,6 +566,9 @@
   <si>
     <t>Figure A3.1: Percentage of last six months of life spent at home or in a community setting</t>
   </si>
+  <si>
+    <t>Figure A3.1: Percentage of time in the last six months of life spent at home or in a community setting; Comparison to old measure</t>
+  </si>
 </sst>
 </file>
 
@@ -1063,6 +1066,9 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1095,9 +1101,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -3196,13 +3199,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3993,7 +3996,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB73"/>
+  <dimension ref="A1:AB74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4194,20 +4197,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
     </row>
     <row r="2" spans="1:28" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
@@ -4494,23 +4497,25 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
+      <c r="B11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="27"/>
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
@@ -4524,23 +4529,21 @@
       <c r="AA11" s="22"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
-      <c r="B12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="28"/>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
@@ -4558,8 +4561,8 @@
     </row>
     <row r="13" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
-      <c r="B13" s="30" t="s">
-        <v>81</v>
+      <c r="B13" s="27" t="s">
+        <v>83</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -4590,7 +4593,9 @@
     </row>
     <row r="14" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+      <c r="B14" s="30" t="s">
+        <v>81</v>
+      </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -4620,9 +4625,7 @@
     </row>
     <row r="15" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
-      <c r="B15" s="31" t="s">
-        <v>74</v>
-      </c>
+      <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -4652,7 +4655,9 @@
     </row>
     <row r="16" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22"/>
-      <c r="B16" s="31"/>
+      <c r="B16" s="31" t="s">
+        <v>74</v>
+      </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -4680,28 +4685,23 @@
       <c r="AA16" s="22"/>
       <c r="AB16" s="22"/>
     </row>
-    <row r="17" spans="1:28" s="24" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
-      <c r="B17" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="112" t="e">
-        <f ca="1">"Hospital data and National Records of Scotland deaths data are provisional for " &amp; [0]!fy_max &amp; ". This publication will be updated in October 20" &amp; RIGHT([0]!fy_max, 2) &amp; " with final figures.  " &amp; "Figures for the latest year should therefore be treated with caution as there could be an undercount of hospital admissions, particularly for people who died in the last three months of the year.  " &amp; "This is not expected to have a large impact on these published figures when they are revised in subsequent updates. "</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="113"/>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="113"/>
-      <c r="N17" s="113"/>
-      <c r="O17" s="113"/>
-      <c r="P17" s="113"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
@@ -4715,23 +4715,28 @@
       <c r="AA17" s="22"/>
       <c r="AB17" s="22"/>
     </row>
-    <row r="18" spans="1:28" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="24" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
+      <c r="B18" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="113" t="e">
+        <f ca="1">"Hospital data and National Records of Scotland deaths data are provisional for " &amp; [0]!fy_max &amp; ". This publication will be updated in October 20" &amp; RIGHT([0]!fy_max, 2) &amp; " with final figures.  " &amp; "Figures for the latest year should therefore be treated with caution as there could be an undercount of hospital admissions, particularly for people who died in the last three months of the year.  " &amp; "This is not expected to have a large impact on these published figures when they are revised in subsequent updates. "</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D18" s="114"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="114"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="114"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
@@ -4745,23 +4750,23 @@
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -4775,43 +4780,56 @@
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32" t="s">
+    <row r="20" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+    </row>
+    <row r="21" spans="1:28" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="110" t="s">
+      <c r="C21" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-    </row>
-    <row r="21" spans="1:28" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
     </row>
     <row r="22" spans="1:28" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="32"/>
@@ -5137,12 +5155,8 @@
       <c r="P40" s="33"/>
     </row>
     <row r="41" spans="2:16" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>77</v>
-      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
@@ -5158,8 +5172,12 @@
       <c r="P41" s="33"/>
     </row>
     <row r="42" spans="2:16" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="32"/>
-      <c r="C42" s="33"/>
+      <c r="B42" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>77</v>
+      </c>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
@@ -5174,88 +5192,104 @@
       <c r="O42" s="33"/>
       <c r="P42" s="33"/>
     </row>
-    <row r="43" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="44" t="s">
+    <row r="43" spans="2:16" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="32"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+    </row>
+    <row r="44" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C44" s="22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="45"/>
-      <c r="C44" s="38" t="s">
+    <row r="45" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="45"/>
+      <c r="C45" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-    </row>
-    <row r="45" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="46"/>
-      <c r="C45" s="35" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="46"/>
+      <c r="C46" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="37"/>
-    </row>
-    <row r="46" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
     </row>
     <row r="47" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="45" t="s">
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="C48" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="2:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B48" s="47"/>
-      <c r="C48" s="33"/>
-    </row>
-    <row r="49" spans="1:16" s="22" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="32"/>
-      <c r="B49" s="48" t="s">
+    <row r="49" spans="1:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B49" s="47"/>
+      <c r="C49" s="33"/>
+    </row>
+    <row r="50" spans="1:16" s="22" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32"/>
+      <c r="B50" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="110" t="s">
+      <c r="C50" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="110"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="110"/>
-      <c r="P49" s="110"/>
-    </row>
-    <row r="50" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-    </row>
-    <row r="51" spans="1:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B51" s="48"/>
-    </row>
-    <row r="52" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="111"/>
+      <c r="L50" s="111"/>
+      <c r="M50" s="111"/>
+      <c r="N50" s="111"/>
+      <c r="O50" s="111"/>
+      <c r="P50" s="111"/>
+    </row>
+    <row r="51" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+    </row>
+    <row r="52" spans="1:16" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="48"/>
+    </row>
     <row r="53" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -5277,22 +5311,24 @@
     <row r="71" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="72" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="73" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C20:P20"/>
-    <mergeCell ref="C49:P49"/>
+    <mergeCell ref="C21:P21"/>
+    <mergeCell ref="C50:P50"/>
     <mergeCell ref="B1:O1"/>
-    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="C18:P18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C44" location="'External Causes of Deaths'!A1" display="For full details of the external causes of death which have been omitted, please click here. "/>
-    <hyperlink ref="C44:K44" location="'External Causes of Deaths'!A1" display="For full details of the external causes of death which have been omitted, please click here. "/>
+    <hyperlink ref="C45" location="'External Causes of Deaths'!A1" display="For full details of the external causes of death which have been omitted, please click here. "/>
+    <hyperlink ref="C45:K45" location="'External Causes of Deaths'!A1" display="For full details of the external causes of death which have been omitted, please click here. "/>
     <hyperlink ref="B6:M6" location="'Figure 1'!A1" display="Figure 1: Percentage of time in the last six months of life spent at home or in a community setting (by age and gender)"/>
     <hyperlink ref="B6" location="'Figure 1'!A1" display="Figure 1: Percentage of time in the last six months of life spent at home or in a community setting (2010/11 - 2016/17)"/>
     <hyperlink ref="B7" location="'Figure 2'!A1" display="Figure 2: Percentage of time in the last six months of life spent at home or in a community setting by NHS Board of residence"/>
     <hyperlink ref="B8" location="'Figure 3'!A1" display="Figure 3: Percentage of time in the last six months of life spent at home or in a community setting (by age and gender)"/>
     <hyperlink ref="B9" location="'Figure 4'!A1" display="Figure 4: Percentage of time in the last six months of life spent at home or in a community setting by Deprivation Category"/>
     <hyperlink ref="B10" location="'Figure 5'!A1" display="Figure 5: Percentage of time in the last six months of life spent at home or in a community setting (by Urban/Rural Classification)"/>
+    <hyperlink ref="B11" location="'Figure A3.1'!A1" display="Figure A3.1: Percentage of time in the last six months of life spent at home or in a community setting; Comparison to old measure"/>
   </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
@@ -5317,17 +5353,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="e">
@@ -5423,19 +5459,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
       <c r="O1" s="50"/>
       <c r="P1" s="50"/>
       <c r="Q1" s="50"/>
@@ -5621,17 +5657,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -5708,13 +5744,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
       <c r="I1" s="72"/>
       <c r="J1" s="72"/>
       <c r="K1" s="72"/>
@@ -5742,7 +5778,7 @@
       <c r="C6" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="121" t="s">
+      <c r="D6" s="110" t="s">
         <v>159</v>
       </c>
       <c r="E6" s="42"/>
@@ -6704,10 +6740,10 @@
     </row>
     <row r="24" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="43"/>
-      <c r="B24" s="119" t="s">
+      <c r="B24" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="119"/>
+      <c r="C24" s="120"/>
       <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6884,16 +6920,16 @@
     </row>
     <row r="43" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="43"/>
-      <c r="B43" s="120"/>
-      <c r="C43" s="120"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
       <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="43"/>
-      <c r="B44" s="119" t="s">
+      <c r="B44" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="119"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -29766,7 +29802,7 @@
     </row>
     <row r="1986" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1986" s="63" t="str">
-        <f t="shared" ref="A1986:A2049" si="31">CONCATENATE(B1986, C1986, D1986)</f>
+        <f t="shared" ref="A1986:A2000" si="31">CONCATENATE(B1986, C1986, D1986)</f>
         <v/>
       </c>
       <c r="B1986" s="79"/>
@@ -30289,17 +30325,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -30376,13 +30412,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
       <c r="I1" s="72"/>
       <c r="J1" s="72"/>
       <c r="K1" s="72"/>
@@ -30405,10 +30441,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="73"/>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="115"/>
+      <c r="D6" s="116"/>
       <c r="E6" s="42"/>
       <c r="G6" s="42"/>
     </row>
@@ -30720,18 +30756,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -30820,15 +30856,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
       <c r="K1" s="50"/>
     </row>
     <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -31208,18 +31244,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -31300,15 +31336,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
       <c r="K1" s="50"/>
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
@@ -31334,14 +31370,14 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="Q6" s="53"/>
@@ -31605,18 +31641,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="e">
@@ -31686,20 +31722,20 @@
       </c>
     </row>
     <row r="36" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="118"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="118"/>
-      <c r="K36" s="118"/>
-      <c r="L36" s="118"/>
-      <c r="M36" s="118"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="119"/>
+      <c r="F36" s="119"/>
+      <c r="G36" s="119"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="119"/>
+      <c r="J36" s="119"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="119"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="59" t="s">
@@ -31767,21 +31803,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="Q1" s="50"/>
       <c r="R1" s="50"/>
       <c r="S1" s="50"/>
@@ -31975,15 +32011,15 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="118" t="str">
+      <c r="B20" s="119" t="str">
         <f>'Figure 4'!B36:M36</f>
         <v>2. Data are analysed by the 2016 ‘Scotland level’ Scottish Index of Multiple Deprivation (SIMD) population weighted quintiles. Each quintile consists of approximately 20% of the population living in Scotland, with deprivation quintile 1 indicating the population living in the most deprived areas.</v>
       </c>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
       <c r="H20" s="62"/>
       <c r="I20" s="62"/>
       <c r="J20" s="62"/>

</xml_diff>